<commit_message>
fixed the issues with database
Signed-off-by: Coca Georgiana <cocageorgiana@gmail.com>
</commit_message>
<xml_diff>
--- a/middleware/StudentsExcel.xlsx
+++ b/middleware/StudentsExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Port</t>
+  </si>
+  <si>
+    <t>popescu</t>
+  </si>
+  <si>
+    <t>ionel</t>
+  </si>
+  <si>
+    <t>8.0</t>
   </si>
 </sst>
 </file>
@@ -205,6 +214,29 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
created integration test with database module
</commit_message>
<xml_diff>
--- a/middleware/StudentsExcel.xlsx
+++ b/middleware/StudentsExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>Id</t>
   </si>
@@ -35,10 +35,10 @@
     <t>Clasificare</t>
   </si>
   <si>
-    <t>Irinel</t>
-  </si>
-  <si>
-    <t>Ionescu</t>
+    <t>Ciprian-Gabriel</t>
+  </si>
+  <si>
+    <t>Cusmuliuc</t>
   </si>
   <si>
     <t>10.0</t>
@@ -47,10 +47,10 @@
     <t>budget</t>
   </si>
   <si>
-    <t>Gigel</t>
-  </si>
-  <si>
-    <t>Popescu</t>
+    <t>Ionel</t>
+  </si>
+  <si>
+    <t>Port</t>
   </si>
   <si>
     <t>9.0</t>
@@ -59,10 +59,28 @@
     <t>9.5</t>
   </si>
   <si>
-    <t>Ionel</t>
-  </si>
-  <si>
-    <t>Port</t>
+    <t>Vasile</t>
+  </si>
+  <si>
+    <t>Grigore</t>
+  </si>
+  <si>
+    <t>8.45</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>8.825</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>fee</t>
   </si>
   <si>
     <t>popescu</t>
@@ -71,7 +89,58 @@
     <t>ionel</t>
   </si>
   <si>
-    <t>8.0</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test now 2</t>
+  </si>
+  <si>
+    <t>6.98</t>
+  </si>
+  <si>
+    <t>7.99</t>
+  </si>
+  <si>
+    <t>Mircea</t>
+  </si>
+  <si>
+    <t>Mihai</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>test now</t>
+  </si>
+  <si>
+    <t>7.49</t>
+  </si>
+  <si>
+    <t>respins</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>Dorian</t>
+  </si>
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>test nou</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>3.495</t>
   </si>
 </sst>
 </file>
@@ -147,7 +216,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4.0</v>
+        <v>18.0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -170,7 +239,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -193,7 +262,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -202,13 +271,13 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -216,25 +285,255 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>